<commit_message>
Fix Test Input. Add Geocode by Amap. Add Staticimage by Baidu.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555DB59E-D9B7-4A96-B6D1-18C896E437D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BC0E30-6F6E-4648-A9A8-C06D99FD5A4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,7 +292,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>河北省石家庄</t>
+    <t>河北省石家庄市</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -637,7 +637,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Fix Staticimage labels by Baidu. Add Staticimage by Amap.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BC0E30-6F6E-4648-A9A8-C06D99FD5A4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FC7898-1EEE-44ED-9D66-C1F4C0AFCCE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="city" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
   <si>
     <t>住址</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,9 +72,6 @@
     <t>租婚庆公司婚车</t>
   </si>
   <si>
-    <t>伯爵宫皇家婚礼会馆</t>
-  </si>
-  <si>
     <t>仓兴街盛邦花园六区</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -170,9 +167,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>盛邦花园六区</t>
-  </si>
-  <si>
     <t>岳父家就餐</t>
   </si>
   <si>
@@ -211,88 +205,105 @@
     <t>核酸检测呈阳性</t>
   </si>
   <si>
+    <t>120负压救护车转运</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核酸复核</t>
+  </si>
+  <si>
+    <t>核酸复核呈阳性，当日诊断为确诊病例</t>
+  </si>
+  <si>
+    <t>裕华区天海誉天下小区A区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12月27至12月30日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12月31日下午</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1月2日中午</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1月2日下午15:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1月2日下午</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1月7日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1月8日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remarks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>河北省石家庄市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>富强大街伯爵宫皇家婚礼会馆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仓兴街盛邦花园六区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>河北省胸科医院</t>
-  </si>
-  <si>
-    <t>120负压救护车转运</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>核酸复核</t>
-  </si>
-  <si>
-    <t>核酸复核呈阳性，当日诊断为确诊病例</t>
-  </si>
-  <si>
-    <t>裕华区天海誉天下小区A区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12月27至12月30日</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12月31日下午</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1月2日中午</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1月2日下午15:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1月2日下午</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1月7日</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1月8日</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>remarks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>city</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>河北省石家庄市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>神州七星酒店</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1月5日中午</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -636,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -647,12 +658,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -674,10 +685,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
@@ -685,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -694,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -708,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC2BAF6-36FA-4FAD-9439-C1542FA46618}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -722,19 +733,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -751,7 +762,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -769,7 +780,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -781,13 +792,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -796,7 +807,7 @@
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -805,7 +816,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -814,7 +825,7 @@
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -823,10 +834,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -843,7 +854,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -870,16 +881,16 @@
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -888,16 +899,16 @@
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -906,13 +917,13 @@
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -924,16 +935,16 @@
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -942,16 +953,16 @@
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -960,7 +971,7 @@
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
@@ -978,16 +989,16 @@
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -996,7 +1007,7 @@
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>0</v>
@@ -1014,16 +1025,16 @@
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1032,16 +1043,16 @@
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1050,16 +1061,16 @@
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1068,7 +1079,7 @@
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>0</v>
@@ -1080,7 +1091,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1088,19 +1099,19 @@
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1108,19 +1119,19 @@
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1128,19 +1139,19 @@
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1148,19 +1159,19 @@
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1169,5 +1180,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>